<commit_message>
Add Prompt and basic datasets evaluation
</commit_message>
<xml_diff>
--- a/Research/Results/PROMPTS/Prompt.xlsx
+++ b/Research/Results/PROMPTS/Prompt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osins\Desktop\AMU-Master-Thesis-Project\Research\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osins\Desktop\AMU-Master-Thesis-Project\Research\Results\PROMPTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88585727-AA3E-4010-A5DB-E61F2897AAE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5469067D-93A4-4217-87FD-0EAF0FFD052A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14685" yWindow="0" windowWidth="14220" windowHeight="15585" tabRatio="592" activeTab="2" xr2:uid="{50ED6178-4609-4BB2-9EEF-E5C268DCCA04}"/>
+    <workbookView xWindow="15120" yWindow="0" windowWidth="13785" windowHeight="15585" tabRatio="592" xr2:uid="{50ED6178-4609-4BB2-9EEF-E5C268DCCA04}"/>
   </bookViews>
   <sheets>
     <sheet name="Prompts" sheetId="5" r:id="rId1"/>
@@ -174,28 +174,13 @@
     <t>#</t>
   </si>
   <si>
-    <t>"</t>
-  </si>
-  <si>
-    <t>'</t>
-  </si>
-  <si>
     <t>###</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>Std</t>
   </si>
   <si>
     <t>&lt;task&gt;</t>
   </si>
   <si>
     <t>&lt;task&gt; benchmark</t>
-  </si>
-  <si>
-    <t>benchmark &lt;task&gt;</t>
   </si>
   <si>
     <t>Relevant concept:</t>
@@ -238,6 +223,21 @@
   </si>
   <si>
     <t>Verified reference:</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
+  <si>
+    <t>64..65</t>
+  </si>
+  <si>
+    <t>(")</t>
+  </si>
+  <si>
+    <t>('')</t>
+  </si>
+  <si>
+    <t>(*)</t>
   </si>
 </sst>
 </file>
@@ -322,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -335,7 +335,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -674,11 +683,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{742E4177-CA9C-4411-B8C3-65C6D789DE87}">
   <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4279,7 +4288,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1:E1048576"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4315,49 +4324,49 @@
         <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -8569,18 +8578,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467AFD9F-315E-4818-998D-C74A3ADBF2AC}">
   <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -8590,23 +8599,23 @@
       <c r="B1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>46</v>
+      <c r="E1" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -8616,14 +8625,24 @@
       <c r="B2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="8">
         <v>43.81</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="D2" s="8">
+        <v>42.89</v>
+      </c>
+      <c r="E2" s="8">
+        <v>41.54</v>
+      </c>
+      <c r="F2" s="8">
+        <v>43.81</v>
+      </c>
+      <c r="G2" s="8">
+        <v>44.19</v>
+      </c>
+      <c r="H2" s="8">
+        <v>43.18</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -8632,14 +8651,24 @@
       <c r="B3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="8">
         <v>21.59</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="D3" s="8">
+        <v>21.08</v>
+      </c>
+      <c r="E3" s="8">
+        <v>21.33</v>
+      </c>
+      <c r="F3" s="8">
+        <v>21.59</v>
+      </c>
+      <c r="G3" s="8">
+        <v>22.01</v>
+      </c>
+      <c r="H3" s="8">
+        <v>21.59</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -8648,14 +8677,24 @@
       <c r="B4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="8">
         <v>23.6</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="D4" s="8">
+        <v>23.31</v>
+      </c>
+      <c r="E4" s="8">
+        <v>23.29</v>
+      </c>
+      <c r="F4" s="8">
+        <v>23.41</v>
+      </c>
+      <c r="G4" s="8">
+        <v>23.46</v>
+      </c>
+      <c r="H4" s="8">
+        <v>23.79</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -8664,14 +8703,24 @@
       <c r="B5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="9">
         <v>51.64</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="D5" s="9">
+        <v>51.22</v>
+      </c>
+      <c r="E5" s="9">
+        <v>50.8</v>
+      </c>
+      <c r="F5" s="9">
+        <v>51.35</v>
+      </c>
+      <c r="G5" s="9">
+        <v>51.14</v>
+      </c>
+      <c r="H5" s="9">
+        <v>51.43</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -8680,14 +8729,24 @@
       <c r="B6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="9">
         <v>22.1</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="D6" s="9">
+        <v>22.78</v>
+      </c>
+      <c r="E6" s="9">
+        <v>22.95</v>
+      </c>
+      <c r="F6" s="9">
+        <v>22.18</v>
+      </c>
+      <c r="G6" s="9">
+        <v>22.27</v>
+      </c>
+      <c r="H6" s="9">
+        <v>21.93</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -8696,14 +8755,24 @@
       <c r="B7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="9">
         <v>22.97</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="D7" s="9">
+        <v>22.96</v>
+      </c>
+      <c r="E7" s="9">
+        <v>22.88</v>
+      </c>
+      <c r="F7" s="9">
+        <v>22.95</v>
+      </c>
+      <c r="G7" s="9">
+        <v>22.9</v>
+      </c>
+      <c r="H7" s="9">
+        <v>22.91</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -8712,14 +8781,24 @@
       <c r="B8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="8">
         <v>63.09</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="D8" s="8">
+        <v>62.92</v>
+      </c>
+      <c r="E8" s="8">
+        <v>62.71</v>
+      </c>
+      <c r="F8" s="8">
+        <v>62.5</v>
+      </c>
+      <c r="G8" s="8">
+        <v>62.58</v>
+      </c>
+      <c r="H8" s="8">
+        <v>62.79</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -8728,14 +8807,24 @@
       <c r="B9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="8">
         <v>26.62</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="D9" s="8">
+        <v>27.56</v>
+      </c>
+      <c r="E9" s="8">
+        <v>27.13</v>
+      </c>
+      <c r="F9" s="8">
+        <v>26.88</v>
+      </c>
+      <c r="G9" s="8">
+        <v>26.88</v>
+      </c>
+      <c r="H9" s="8">
+        <v>27.39</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -8744,14 +8833,24 @@
       <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="8">
         <v>25.25</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="D10" s="8">
+        <v>24.88</v>
+      </c>
+      <c r="E10" s="8">
+        <v>24.64</v>
+      </c>
+      <c r="F10" s="8">
+        <v>25.6</v>
+      </c>
+      <c r="G10" s="8">
+        <v>25.67</v>
+      </c>
+      <c r="H10" s="8">
+        <v>25.24</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -8760,14 +8859,24 @@
       <c r="B11" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="9">
         <v>69.7</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+      <c r="D11" s="9">
+        <v>70.08</v>
+      </c>
+      <c r="E11" s="9">
+        <v>69.739999999999995</v>
+      </c>
+      <c r="F11" s="9">
+        <v>69.61</v>
+      </c>
+      <c r="G11" s="9">
+        <v>68.86</v>
+      </c>
+      <c r="H11" s="9">
+        <v>70.03</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -8776,14 +8885,24 @@
       <c r="B12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="9">
         <v>36.26</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+      <c r="D12" s="9">
+        <v>36.35</v>
+      </c>
+      <c r="E12" s="9">
+        <v>36.43</v>
+      </c>
+      <c r="F12" s="9">
+        <v>36.520000000000003</v>
+      </c>
+      <c r="G12" s="9">
+        <v>35.92</v>
+      </c>
+      <c r="H12" s="9">
+        <v>36.01</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -8792,14 +8911,24 @@
       <c r="B13" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="9">
         <v>50.05</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+      <c r="D13" s="9">
+        <v>49.99</v>
+      </c>
+      <c r="E13" s="9">
+        <v>49.99</v>
+      </c>
+      <c r="F13" s="9">
+        <v>50.2</v>
+      </c>
+      <c r="G13" s="9">
+        <v>50.19</v>
+      </c>
+      <c r="H13" s="9">
+        <v>49.63</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -8808,14 +8937,24 @@
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="8">
         <v>68.86</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="D14" s="8">
+        <v>68.010000000000005</v>
+      </c>
+      <c r="E14" s="8">
+        <v>68.349999999999994</v>
+      </c>
+      <c r="F14" s="8">
+        <v>68.81</v>
+      </c>
+      <c r="G14" s="8">
+        <v>68.81</v>
+      </c>
+      <c r="H14" s="8">
+        <v>68.56</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -8824,14 +8963,24 @@
       <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="8">
         <v>34.47</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="D15" s="8">
+        <v>33.96</v>
+      </c>
+      <c r="E15" s="8">
+        <v>34.22</v>
+      </c>
+      <c r="F15" s="8">
+        <v>34.56</v>
+      </c>
+      <c r="G15" s="8">
+        <v>34.9</v>
+      </c>
+      <c r="H15" s="8">
+        <v>34.729999999999997</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -8840,14 +8989,24 @@
       <c r="B16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="8">
         <v>40.54</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+      <c r="D16" s="8">
+        <v>40.479999999999997</v>
+      </c>
+      <c r="E16" s="8">
+        <v>39.840000000000003</v>
+      </c>
+      <c r="F16" s="8">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="G16" s="8">
+        <v>40.340000000000003</v>
+      </c>
+      <c r="H16" s="8">
+        <v>40.619999999999997</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -8856,14 +9015,24 @@
       <c r="B17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="9">
         <v>65.91</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
+      <c r="D17" s="9">
+        <v>65.569999999999993</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="9">
+        <v>65.489999999999995</v>
+      </c>
+      <c r="G17" s="9">
+        <v>65.87</v>
+      </c>
+      <c r="H17" s="9">
+        <v>65.53</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -8872,14 +9041,24 @@
       <c r="B18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="9">
         <v>34.130000000000003</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+      <c r="D18" s="9">
+        <v>31.48</v>
+      </c>
+      <c r="E18" s="9">
+        <v>31.48</v>
+      </c>
+      <c r="F18" s="9">
+        <v>31.83</v>
+      </c>
+      <c r="G18" s="9">
+        <v>31.74</v>
+      </c>
+      <c r="H18" s="9">
+        <v>32.51</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
@@ -8888,14 +9067,24 @@
       <c r="B19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="9">
         <v>25.62</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
+      <c r="D19" s="9">
+        <v>25.62</v>
+      </c>
+      <c r="E19" s="9">
+        <v>25.45</v>
+      </c>
+      <c r="F19" s="9">
+        <v>25.72</v>
+      </c>
+      <c r="G19" s="9">
+        <v>25.47</v>
+      </c>
+      <c r="H19" s="9">
+        <v>25.64</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -8904,14 +9093,24 @@
       <c r="B20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="8">
         <v>66.12</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="D20" s="8">
+        <v>65.11</v>
+      </c>
+      <c r="E20" s="8">
+        <v>67.09</v>
+      </c>
+      <c r="F20" s="8">
+        <v>66.58</v>
+      </c>
+      <c r="G20" s="8">
+        <v>64.52</v>
+      </c>
+      <c r="H20" s="8">
+        <v>62.04</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -8920,14 +9119,24 @@
       <c r="B21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="8">
         <v>38.229999999999997</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="D21" s="8">
+        <v>38.049999999999997</v>
+      </c>
+      <c r="E21" s="8">
+        <v>38.909999999999997</v>
+      </c>
+      <c r="F21" s="8">
+        <v>39.93</v>
+      </c>
+      <c r="G21" s="8">
+        <v>38.229999999999997</v>
+      </c>
+      <c r="H21" s="8">
+        <v>37.46</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -8936,14 +9145,24 @@
       <c r="B22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="8">
         <v>50.33</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="D22" s="8">
+        <v>49.59</v>
+      </c>
+      <c r="E22" s="8">
+        <v>49.51</v>
+      </c>
+      <c r="F22" s="8">
+        <v>50.19</v>
+      </c>
+      <c r="G22" s="8">
+        <v>49.9</v>
+      </c>
+      <c r="H22" s="8">
+        <v>49.7</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
@@ -8952,14 +9171,24 @@
       <c r="B23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="9">
         <v>77.02</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
+      <c r="D23" s="9">
+        <v>76.64</v>
+      </c>
+      <c r="E23" s="9">
+        <v>76.010000000000005</v>
+      </c>
+      <c r="F23" s="9">
+        <v>76.77</v>
+      </c>
+      <c r="G23" s="9">
+        <v>76.52</v>
+      </c>
+      <c r="H23" s="9">
+        <v>77.02</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -8968,14 +9197,24 @@
       <c r="B24" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="9">
         <v>43</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+      <c r="D24" s="9">
+        <v>41.98</v>
+      </c>
+      <c r="E24" s="9">
+        <v>43.09</v>
+      </c>
+      <c r="F24" s="9">
+        <v>43.17</v>
+      </c>
+      <c r="G24" s="9">
+        <v>42.66</v>
+      </c>
+      <c r="H24" s="9">
+        <v>42.75</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -8984,14 +9223,24 @@
       <c r="B25" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="9">
         <v>49.72</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
+      <c r="D25" s="9">
+        <v>49.7</v>
+      </c>
+      <c r="E25" s="9">
+        <v>49.41</v>
+      </c>
+      <c r="F25" s="9">
+        <v>49.9</v>
+      </c>
+      <c r="G25" s="9">
+        <v>49.39</v>
+      </c>
+      <c r="H25" s="9">
+        <v>49.44</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -9000,14 +9249,24 @@
       <c r="B26" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="8">
         <v>75.13</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="D26" s="8">
+        <v>74.75</v>
+      </c>
+      <c r="E26" s="8">
+        <v>73.7</v>
+      </c>
+      <c r="F26" s="8">
+        <v>74.41</v>
+      </c>
+      <c r="G26" s="8">
+        <v>74.239999999999995</v>
+      </c>
+      <c r="H26" s="8">
+        <v>74.92</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
@@ -9016,14 +9275,24 @@
       <c r="B27" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="8">
         <v>45.56</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="D27" s="8">
+        <v>44.11</v>
+      </c>
+      <c r="E27" s="8">
+        <v>44.03</v>
+      </c>
+      <c r="F27" s="8">
+        <v>43.86</v>
+      </c>
+      <c r="G27" s="8">
+        <v>43.17</v>
+      </c>
+      <c r="H27" s="8">
+        <v>45.05</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
@@ -9032,14 +9301,24 @@
       <c r="B28" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="8">
         <v>60.86</v>
       </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
+      <c r="D28" s="8">
+        <v>60.79</v>
+      </c>
+      <c r="E28" s="8">
+        <v>60.6</v>
+      </c>
+      <c r="F28" s="8">
+        <v>60.88</v>
+      </c>
+      <c r="G28" s="8">
+        <v>60.75</v>
+      </c>
+      <c r="H28" s="8">
+        <v>60.89</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
@@ -9048,14 +9327,24 @@
       <c r="B29" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="9">
         <v>74.62</v>
       </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
+      <c r="D29" s="9">
+        <v>74.959999999999994</v>
+      </c>
+      <c r="E29" s="9">
+        <v>73.95</v>
+      </c>
+      <c r="F29" s="9">
+        <v>74.83</v>
+      </c>
+      <c r="G29" s="9">
+        <v>74.709999999999994</v>
+      </c>
+      <c r="H29" s="9">
+        <v>74.12</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
@@ -9064,14 +9353,24 @@
       <c r="B30" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="9">
         <v>43.34</v>
       </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
+      <c r="D30" s="9">
+        <v>43.17</v>
+      </c>
+      <c r="E30" s="9">
+        <v>42.49</v>
+      </c>
+      <c r="F30" s="9">
+        <v>42.92</v>
+      </c>
+      <c r="G30" s="9">
+        <v>42.92</v>
+      </c>
+      <c r="H30" s="9">
+        <v>42.75</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
@@ -9080,14 +9379,24 @@
       <c r="B31" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="9">
         <v>60.66</v>
       </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
+      <c r="D31" s="9">
+        <v>60.72</v>
+      </c>
+      <c r="E31" s="9">
+        <v>60.65</v>
+      </c>
+      <c r="F31" s="9">
+        <v>60.6</v>
+      </c>
+      <c r="G31" s="9">
+        <v>60.63</v>
+      </c>
+      <c r="H31" s="9">
+        <v>60.68</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
@@ -9096,14 +9405,24 @@
       <c r="B32" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="8">
         <v>78.489999999999995</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
+      <c r="D32" s="8">
+        <v>76.849999999999994</v>
+      </c>
+      <c r="E32" s="8">
+        <v>77.06</v>
+      </c>
+      <c r="F32" s="8">
+        <v>77.569999999999993</v>
+      </c>
+      <c r="G32" s="8">
+        <v>77.53</v>
+      </c>
+      <c r="H32" s="8">
+        <v>77.48</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
@@ -9112,14 +9431,24 @@
       <c r="B33" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="8">
         <v>45.48</v>
       </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
+      <c r="D33" s="8">
+        <v>44.8</v>
+      </c>
+      <c r="E33" s="8">
+        <v>42.92</v>
+      </c>
+      <c r="F33" s="8">
+        <v>45.9</v>
+      </c>
+      <c r="G33" s="8">
+        <v>45.48</v>
+      </c>
+      <c r="H33" s="8">
+        <v>43.69</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
@@ -9128,14 +9457,24 @@
       <c r="B34" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="8">
         <v>51.25</v>
       </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
+      <c r="D34" s="8">
+        <v>51.01</v>
+      </c>
+      <c r="E34" s="8">
+        <v>51.33</v>
+      </c>
+      <c r="F34" s="8">
+        <v>51.53</v>
+      </c>
+      <c r="G34" s="8">
+        <v>51.11</v>
+      </c>
+      <c r="H34" s="8">
+        <v>51.6</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
@@ -9144,14 +9483,24 @@
       <c r="B35" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="9">
         <v>78.87</v>
       </c>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
+      <c r="D35" s="9">
+        <v>78.41</v>
+      </c>
+      <c r="E35" s="9">
+        <v>77.86</v>
+      </c>
+      <c r="F35" s="9">
+        <v>78.16</v>
+      </c>
+      <c r="G35" s="9">
+        <v>78.540000000000006</v>
+      </c>
+      <c r="H35" s="9">
+        <v>78.540000000000006</v>
+      </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
@@ -9160,14 +9509,24 @@
       <c r="B36" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="9">
         <v>47.78</v>
       </c>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
+      <c r="D36" s="9">
+        <v>46.16</v>
+      </c>
+      <c r="E36" s="9">
+        <v>45.9</v>
+      </c>
+      <c r="F36" s="9">
+        <v>47.27</v>
+      </c>
+      <c r="G36" s="9">
+        <v>47.1</v>
+      </c>
+      <c r="H36" s="9">
+        <v>46.84</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
@@ -9176,14 +9535,24 @@
       <c r="B37" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="9">
         <v>58.55</v>
       </c>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
+      <c r="D37" s="9">
+        <v>58.41</v>
+      </c>
+      <c r="E37" s="9">
+        <v>58.5</v>
+      </c>
+      <c r="F37" s="9">
+        <v>58.52</v>
+      </c>
+      <c r="G37" s="9">
+        <v>58.44</v>
+      </c>
+      <c r="H37" s="9">
+        <v>58.56</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
@@ -9192,14 +9561,24 @@
       <c r="B38" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="8">
         <v>76.09</v>
       </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
+      <c r="D38" s="8">
+        <v>75.55</v>
+      </c>
+      <c r="E38" s="8">
+        <v>75.88</v>
+      </c>
+      <c r="F38" s="8">
+        <v>75.8</v>
+      </c>
+      <c r="G38" s="8">
+        <v>76.05</v>
+      </c>
+      <c r="H38" s="8">
+        <v>76.260000000000005</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
@@ -9208,14 +9587,24 @@
       <c r="B39" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="8">
         <v>44.8</v>
       </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
+      <c r="D39" s="8">
+        <v>45.31</v>
+      </c>
+      <c r="E39" s="8">
+        <v>44.28</v>
+      </c>
+      <c r="F39" s="8">
+        <v>44.8</v>
+      </c>
+      <c r="G39" s="8">
+        <v>44.97</v>
+      </c>
+      <c r="H39" s="8">
+        <v>44.88</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -9224,14 +9613,24 @@
       <c r="B40" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="8">
         <v>62.35</v>
       </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
+      <c r="D40" s="8">
+        <v>61.7</v>
+      </c>
+      <c r="E40" s="8">
+        <v>62.3</v>
+      </c>
+      <c r="F40" s="8">
+        <v>61.79</v>
+      </c>
+      <c r="G40" s="8">
+        <v>62.11</v>
+      </c>
+      <c r="H40" s="8">
+        <v>62.09</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
@@ -9240,14 +9639,24 @@
       <c r="B41" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C41" s="9">
         <v>76.81</v>
       </c>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
+      <c r="D41" s="9">
+        <v>75.55</v>
+      </c>
+      <c r="E41" s="9">
+        <v>75.88</v>
+      </c>
+      <c r="F41" s="9">
+        <v>75.8</v>
+      </c>
+      <c r="G41" s="9">
+        <v>76.05</v>
+      </c>
+      <c r="H41" s="9">
+        <v>76.260000000000005</v>
+      </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
@@ -9256,14 +9665,24 @@
       <c r="B42" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="9">
         <v>42.58</v>
       </c>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
+      <c r="D42" s="9">
+        <v>45.31</v>
+      </c>
+      <c r="E42" s="9">
+        <v>44.28</v>
+      </c>
+      <c r="F42" s="9">
+        <v>44.8</v>
+      </c>
+      <c r="G42" s="9">
+        <v>44.97</v>
+      </c>
+      <c r="H42" s="9">
+        <v>44.88</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
@@ -9272,14 +9691,24 @@
       <c r="B43" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C43" s="9">
         <v>56.25</v>
       </c>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
+      <c r="D43" s="9">
+        <v>61.7</v>
+      </c>
+      <c r="E43" s="9">
+        <v>62.3</v>
+      </c>
+      <c r="F43" s="9">
+        <v>61.79</v>
+      </c>
+      <c r="G43" s="9">
+        <v>62.11</v>
+      </c>
+      <c r="H43" s="9">
+        <v>62.09</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
@@ -9288,14 +9717,24 @@
       <c r="B44" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="8">
         <v>77.78</v>
       </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
+      <c r="D44" s="8">
+        <v>77.86</v>
+      </c>
+      <c r="E44" s="8">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="F44" s="8">
+        <v>78.28</v>
+      </c>
+      <c r="G44" s="8">
+        <v>78.45</v>
+      </c>
+      <c r="H44" s="8">
+        <v>77.31</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
@@ -9304,14 +9743,24 @@
       <c r="B45" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="8">
         <v>47.35</v>
       </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
+      <c r="D45" s="8">
+        <v>46.67</v>
+      </c>
+      <c r="E45" s="8">
+        <v>45.99</v>
+      </c>
+      <c r="F45" s="8">
+        <v>46.76</v>
+      </c>
+      <c r="G45" s="8">
+        <v>46.93</v>
+      </c>
+      <c r="H45" s="8">
+        <v>47.18</v>
+      </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
@@ -9320,14 +9769,24 @@
       <c r="B46" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="8">
         <v>65.47</v>
       </c>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
+      <c r="D46" s="8">
+        <v>65.52</v>
+      </c>
+      <c r="E46" s="8">
+        <v>65.58</v>
+      </c>
+      <c r="F46" s="8">
+        <v>65.67</v>
+      </c>
+      <c r="G46" s="8">
+        <v>65.64</v>
+      </c>
+      <c r="H46" s="8">
+        <v>65.489999999999995</v>
+      </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
@@ -9336,14 +9795,24 @@
       <c r="B47" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="9">
         <v>75.88</v>
       </c>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
+      <c r="D47" s="9">
+        <v>73.27</v>
+      </c>
+      <c r="E47" s="9">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="F47" s="9">
+        <v>76.349999999999994</v>
+      </c>
+      <c r="G47" s="9">
+        <v>76.349999999999994</v>
+      </c>
+      <c r="H47" s="9">
+        <v>74.58</v>
+      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
@@ -9352,14 +9821,24 @@
       <c r="B48" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C48" s="9">
         <v>44.54</v>
       </c>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
+      <c r="D48" s="9">
+        <v>42.58</v>
+      </c>
+      <c r="E48" s="9">
+        <v>43.09</v>
+      </c>
+      <c r="F48" s="9">
+        <v>46.33</v>
+      </c>
+      <c r="G48" s="9">
+        <v>46.08</v>
+      </c>
+      <c r="H48" s="9">
+        <v>44.88</v>
+      </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
@@ -9368,14 +9847,24 @@
       <c r="B49" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C49" s="9">
         <v>66.73</v>
       </c>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
+      <c r="D49" s="9">
+        <v>66.239999999999995</v>
+      </c>
+      <c r="E49" s="9">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="F49" s="9">
+        <v>66.34</v>
+      </c>
+      <c r="G49" s="9">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="H49" s="9">
+        <v>66.22</v>
+      </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
@@ -9384,14 +9873,24 @@
       <c r="B50" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50" s="8">
         <v>82.79</v>
       </c>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
+      <c r="D50" s="8">
+        <v>82.32</v>
+      </c>
+      <c r="E50" s="8">
+        <v>80.81</v>
+      </c>
+      <c r="F50" s="8">
+        <v>82.74</v>
+      </c>
+      <c r="G50" s="8">
+        <v>82.62</v>
+      </c>
+      <c r="H50" s="8">
+        <v>83.04</v>
+      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
@@ -9400,14 +9899,24 @@
       <c r="B51" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51" s="8">
         <v>57.42</v>
       </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
+      <c r="D51" s="8">
+        <v>57.08</v>
+      </c>
+      <c r="E51" s="8">
+        <v>55.89</v>
+      </c>
+      <c r="F51" s="8">
+        <v>57.25</v>
+      </c>
+      <c r="G51" s="8">
+        <v>56.83</v>
+      </c>
+      <c r="H51" s="8">
+        <v>57.51</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
@@ -9416,14 +9925,24 @@
       <c r="B52" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52" s="8">
         <v>69.62</v>
       </c>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
+      <c r="D52" s="8">
+        <v>69.53</v>
+      </c>
+      <c r="E52" s="8">
+        <v>69.64</v>
+      </c>
+      <c r="F52" s="8">
+        <v>69.69</v>
+      </c>
+      <c r="G52" s="8">
+        <v>69.48</v>
+      </c>
+      <c r="H52" s="8">
+        <v>69.73</v>
+      </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
@@ -9432,14 +9951,24 @@
       <c r="B53" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C53" s="9">
         <v>76.05</v>
       </c>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
+      <c r="D53" s="9">
+        <v>75.209999999999994</v>
+      </c>
+      <c r="E53" s="9">
+        <v>75.459999999999994</v>
+      </c>
+      <c r="F53" s="9">
+        <v>75.55</v>
+      </c>
+      <c r="G53" s="9">
+        <v>75.510000000000005</v>
+      </c>
+      <c r="H53" s="9">
+        <v>75.59</v>
+      </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
@@ -9448,14 +9977,24 @@
       <c r="B54" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C54" s="9">
         <v>42.06</v>
       </c>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
+      <c r="D54" s="9">
+        <v>41.64</v>
+      </c>
+      <c r="E54" s="9">
+        <v>41.21</v>
+      </c>
+      <c r="F54" s="9">
+        <v>41.89</v>
+      </c>
+      <c r="G54" s="9">
+        <v>41.89</v>
+      </c>
+      <c r="H54" s="9">
+        <v>41.81</v>
+      </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
@@ -9464,14 +10003,24 @@
       <c r="B55" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C55" s="9">
         <v>46.99</v>
       </c>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
+      <c r="D55" s="9">
+        <v>47.08</v>
+      </c>
+      <c r="E55" s="9">
+        <v>47.21</v>
+      </c>
+      <c r="F55" s="9">
+        <v>46.94</v>
+      </c>
+      <c r="G55" s="9">
+        <v>46.91</v>
+      </c>
+      <c r="H55" s="9">
+        <v>47.02</v>
+      </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
@@ -9480,14 +10029,24 @@
       <c r="B56" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C56" s="8">
         <v>81.19</v>
       </c>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
+      <c r="D56" s="8">
+        <v>80.010000000000005</v>
+      </c>
+      <c r="E56" s="8">
+        <v>80.47</v>
+      </c>
+      <c r="F56" s="8">
+        <v>79.63</v>
+      </c>
+      <c r="G56" s="8">
+        <v>79.97</v>
+      </c>
+      <c r="H56" s="8">
+        <v>80.3</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
@@ -9496,14 +10055,24 @@
       <c r="B57" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C57" s="3">
+      <c r="C57" s="8">
         <v>55.12</v>
       </c>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
+      <c r="D57" s="8">
+        <v>52.22</v>
+      </c>
+      <c r="E57" s="8">
+        <v>54.52</v>
+      </c>
+      <c r="F57" s="8">
+        <v>53.92</v>
+      </c>
+      <c r="G57" s="8">
+        <v>52.99</v>
+      </c>
+      <c r="H57" s="8">
+        <v>54.01</v>
+      </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
@@ -9512,14 +10081,24 @@
       <c r="B58" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C58" s="3">
+      <c r="C58" s="8">
         <v>61.53</v>
       </c>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
+      <c r="D58" s="8">
+        <v>61.34</v>
+      </c>
+      <c r="E58" s="8">
+        <v>61.31</v>
+      </c>
+      <c r="F58" s="8">
+        <v>61.44</v>
+      </c>
+      <c r="G58" s="8">
+        <v>61.2</v>
+      </c>
+      <c r="H58" s="8">
+        <v>61.39</v>
+      </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
@@ -9528,14 +10107,24 @@
       <c r="B59" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C59" s="9">
         <v>80.599999999999994</v>
       </c>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
-      <c r="H59" s="5"/>
+      <c r="D59" s="9">
+        <v>80.39</v>
+      </c>
+      <c r="E59" s="9">
+        <v>80.3</v>
+      </c>
+      <c r="F59" s="9">
+        <v>80.77</v>
+      </c>
+      <c r="G59" s="9">
+        <v>80.89</v>
+      </c>
+      <c r="H59" s="9">
+        <v>80.680000000000007</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
@@ -9544,14 +10133,24 @@
       <c r="B60" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C60" s="9">
         <v>48.12</v>
       </c>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
+      <c r="D60" s="9">
+        <v>47.18</v>
+      </c>
+      <c r="E60" s="9">
+        <v>47.1</v>
+      </c>
+      <c r="F60" s="9">
+        <v>49.23</v>
+      </c>
+      <c r="G60" s="9">
+        <v>49.23</v>
+      </c>
+      <c r="H60" s="9">
+        <v>48.55</v>
+      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
@@ -9560,14 +10159,24 @@
       <c r="B61" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C61" s="9">
         <v>61.02</v>
       </c>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
+      <c r="D61" s="9">
+        <v>61.1</v>
+      </c>
+      <c r="E61" s="9">
+        <v>61.22</v>
+      </c>
+      <c r="F61" s="9">
+        <v>61.13</v>
+      </c>
+      <c r="G61" s="9">
+        <v>60.98</v>
+      </c>
+      <c r="H61" s="9">
+        <v>61.71</v>
+      </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
@@ -9576,14 +10185,24 @@
       <c r="B62" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C62" s="3">
-        <v>8316</v>
-      </c>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
+      <c r="C62" s="8">
+        <v>83.16</v>
+      </c>
+      <c r="D62" s="8">
+        <v>83</v>
+      </c>
+      <c r="E62" s="8">
+        <v>83.08</v>
+      </c>
+      <c r="F62" s="8">
+        <v>83.96</v>
+      </c>
+      <c r="G62" s="8">
+        <v>83.46</v>
+      </c>
+      <c r="H62" s="8">
+        <v>83.54</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
@@ -9592,14 +10211,24 @@
       <c r="B63" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C63" s="3">
+      <c r="C63" s="8">
         <v>53.5</v>
       </c>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
+      <c r="D63" s="8">
+        <v>54.78</v>
+      </c>
+      <c r="E63" s="8">
+        <v>54.95</v>
+      </c>
+      <c r="F63" s="8">
+        <v>55.38</v>
+      </c>
+      <c r="G63" s="8">
+        <v>54.44</v>
+      </c>
+      <c r="H63" s="8">
+        <v>54.52</v>
+      </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
@@ -9608,14 +10237,24 @@
       <c r="B64" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C64" s="3">
+      <c r="C64" s="8">
         <v>61.56</v>
       </c>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
+      <c r="D64" s="8">
+        <v>61.63</v>
+      </c>
+      <c r="E64" s="8">
+        <v>61.71</v>
+      </c>
+      <c r="F64" s="8">
+        <v>61.64</v>
+      </c>
+      <c r="G64" s="8">
+        <v>61.7</v>
+      </c>
+      <c r="H64" s="8">
+        <v>61.69</v>
+      </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
@@ -9624,14 +10263,24 @@
       <c r="B65" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C65" s="9">
         <v>78.91</v>
       </c>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
+      <c r="D65" s="9">
+        <v>78.540000000000006</v>
+      </c>
+      <c r="E65" s="9">
+        <v>76.39</v>
+      </c>
+      <c r="F65" s="9">
+        <v>77.78</v>
+      </c>
+      <c r="G65" s="9">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="H65" s="9">
+        <v>77.61</v>
+      </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
@@ -9640,14 +10289,24 @@
       <c r="B66" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C66" s="9">
         <v>51.96</v>
       </c>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5"/>
-      <c r="H66" s="5"/>
+      <c r="D66" s="9">
+        <v>52.56</v>
+      </c>
+      <c r="E66" s="9">
+        <v>49.74</v>
+      </c>
+      <c r="F66" s="9">
+        <v>51.62</v>
+      </c>
+      <c r="G66" s="9">
+        <v>51.19</v>
+      </c>
+      <c r="H66" s="9">
+        <v>52.22</v>
+      </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
@@ -9656,14 +10315,24 @@
       <c r="B67" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C67" s="9">
         <v>71.81</v>
       </c>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5"/>
+      <c r="D67" s="9">
+        <v>71.72</v>
+      </c>
+      <c r="E67" s="9">
+        <v>71.55</v>
+      </c>
+      <c r="F67" s="9">
+        <v>71.52</v>
+      </c>
+      <c r="G67" s="9">
+        <v>71.73</v>
+      </c>
+      <c r="H67" s="9">
+        <v>71.86</v>
+      </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
@@ -9672,14 +10341,24 @@
       <c r="B68" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C68" s="3">
+      <c r="C68" s="8">
         <v>82.07</v>
       </c>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
+      <c r="D68" s="8">
+        <v>78.540000000000006</v>
+      </c>
+      <c r="E68" s="8">
+        <v>76.39</v>
+      </c>
+      <c r="F68" s="8">
+        <v>77.78</v>
+      </c>
+      <c r="G68" s="8">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="H68" s="8">
+        <v>77.61</v>
+      </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
@@ -9688,14 +10367,24 @@
       <c r="B69" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C69" s="3">
+      <c r="C69" s="8">
         <v>52.65</v>
       </c>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
-      <c r="H69" s="3"/>
+      <c r="D69" s="8">
+        <v>52.56</v>
+      </c>
+      <c r="E69" s="8">
+        <v>49.74</v>
+      </c>
+      <c r="F69" s="8">
+        <v>51.62</v>
+      </c>
+      <c r="G69" s="8">
+        <v>51.19</v>
+      </c>
+      <c r="H69" s="8">
+        <v>52.22</v>
+      </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
@@ -9704,14 +10393,24 @@
       <c r="B70" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C70" s="3">
+      <c r="C70" s="8">
         <v>71.52</v>
       </c>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
+      <c r="D70" s="8">
+        <v>71.72</v>
+      </c>
+      <c r="E70" s="8">
+        <v>71.55</v>
+      </c>
+      <c r="F70" s="8">
+        <v>71.52</v>
+      </c>
+      <c r="G70" s="8">
+        <v>71.73</v>
+      </c>
+      <c r="H70" s="8">
+        <v>71.86</v>
+      </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
@@ -9720,14 +10419,24 @@
       <c r="B71" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C71" s="9">
         <v>81.31</v>
       </c>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5"/>
+      <c r="D71" s="9">
+        <v>80.349999999999994</v>
+      </c>
+      <c r="E71" s="9">
+        <v>80.09</v>
+      </c>
+      <c r="F71" s="9">
+        <v>81.36</v>
+      </c>
+      <c r="G71" s="9">
+        <v>80.930000000000007</v>
+      </c>
+      <c r="H71" s="9">
+        <v>81.14</v>
+      </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
@@ -9736,14 +10445,24 @@
       <c r="B72" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C72" s="9">
         <v>49.4</v>
       </c>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="5"/>
-      <c r="G72" s="5"/>
-      <c r="H72" s="5"/>
+      <c r="D72" s="9">
+        <v>47.95</v>
+      </c>
+      <c r="E72" s="9">
+        <v>46.93</v>
+      </c>
+      <c r="F72" s="9">
+        <v>48.89</v>
+      </c>
+      <c r="G72" s="9">
+        <v>49.06</v>
+      </c>
+      <c r="H72" s="9">
+        <v>49.32</v>
+      </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
@@ -9752,14 +10471,24 @@
       <c r="B73" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C73" s="9">
         <v>62.92</v>
       </c>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
+      <c r="D73" s="9">
+        <v>63.06</v>
+      </c>
+      <c r="E73" s="9">
+        <v>63.14</v>
+      </c>
+      <c r="F73" s="9">
+        <v>63.42</v>
+      </c>
+      <c r="G73" s="9">
+        <v>63.34</v>
+      </c>
+      <c r="H73" s="9">
+        <v>63.24</v>
+      </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
@@ -9768,14 +10497,24 @@
       <c r="B74" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C74" s="3">
+      <c r="C74" s="8">
         <v>81.36</v>
       </c>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
-      <c r="H74" s="3"/>
+      <c r="D74" s="8">
+        <v>80.13</v>
+      </c>
+      <c r="E74" s="8">
+        <v>80.260000000000005</v>
+      </c>
+      <c r="F74" s="8">
+        <v>80.89</v>
+      </c>
+      <c r="G74" s="8">
+        <v>80.89</v>
+      </c>
+      <c r="H74" s="8">
+        <v>80.849999999999994</v>
+      </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
@@ -9784,14 +10523,24 @@
       <c r="B75" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C75" s="3">
+      <c r="C75" s="8">
         <v>51.88</v>
       </c>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
-      <c r="H75" s="3"/>
+      <c r="D75" s="8">
+        <v>51.19</v>
+      </c>
+      <c r="E75" s="8">
+        <v>50.77</v>
+      </c>
+      <c r="F75" s="8">
+        <v>65.87</v>
+      </c>
+      <c r="G75" s="8">
+        <v>65.95</v>
+      </c>
+      <c r="H75" s="8">
+        <v>51.54</v>
+      </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
@@ -9800,14 +10549,24 @@
       <c r="B76" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C76" s="3">
+      <c r="C76" s="8">
         <v>66.099999999999994</v>
       </c>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
-      <c r="G76" s="3"/>
-      <c r="H76" s="3"/>
+      <c r="D76" s="8">
+        <v>65.62</v>
+      </c>
+      <c r="E76" s="8">
+        <v>65.989999999999995</v>
+      </c>
+      <c r="F76" s="8">
+        <v>65.87</v>
+      </c>
+      <c r="G76" s="8">
+        <v>65.95</v>
+      </c>
+      <c r="H76" s="8">
+        <v>65.8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9816,942 +10575,1315 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B9A7D6B-CAE5-41B4-8E9A-54CA3E2B940F}">
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
     <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>48</v>
+      <c r="C1" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C2" s="8">
+        <v>43.81</v>
+      </c>
+      <c r="D2" s="3">
+        <v>43.56</v>
+      </c>
+      <c r="E2" s="3">
+        <v>43.27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="8">
+        <v>21.59</v>
+      </c>
+      <c r="D3" s="3">
+        <v>20.99</v>
+      </c>
+      <c r="E3" s="3">
+        <v>21.59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="8">
+        <v>23.6</v>
+      </c>
+      <c r="D4" s="3">
+        <v>23.59</v>
+      </c>
+      <c r="E4" s="3">
+        <v>23.42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="9">
+        <v>51.64</v>
+      </c>
+      <c r="D5" s="5">
+        <v>51.05</v>
+      </c>
+      <c r="E5" s="5">
+        <v>50.84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="9">
+        <v>22.1</v>
+      </c>
+      <c r="D6" s="5">
+        <v>22.35</v>
+      </c>
+      <c r="E6" s="5">
+        <v>22.53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="9">
+        <v>22.97</v>
+      </c>
+      <c r="D7" s="5">
+        <v>22.92</v>
+      </c>
+      <c r="E7" s="5">
+        <v>22.92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="8">
+        <v>63.09</v>
+      </c>
+      <c r="D8" s="3">
+        <v>62.58</v>
+      </c>
+      <c r="E8" s="3">
+        <v>62.54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="8">
+        <v>26.62</v>
+      </c>
+      <c r="D9" s="3">
+        <v>26.88</v>
+      </c>
+      <c r="E9" s="3">
+        <v>26.62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="8">
+        <v>25.25</v>
+      </c>
+      <c r="D10" s="3">
+        <v>25.99</v>
+      </c>
+      <c r="E10" s="3">
+        <v>25.93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="9">
+        <v>69.7</v>
+      </c>
+      <c r="D11" s="5">
+        <v>70.290000000000006</v>
+      </c>
+      <c r="E11" s="5">
+        <v>69.650000000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="9">
+        <v>36.26</v>
+      </c>
+      <c r="D12" s="5">
+        <v>36.520000000000003</v>
+      </c>
+      <c r="E12" s="5">
+        <v>36.950000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="9">
+        <v>50.05</v>
+      </c>
+      <c r="D13" s="5">
+        <v>50.04</v>
+      </c>
+      <c r="E13" s="5">
+        <v>50.01</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="8">
+        <v>68.86</v>
+      </c>
+      <c r="D14" s="3">
+        <v>68.77</v>
+      </c>
+      <c r="E14" s="3">
+        <v>67.47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="8">
+        <v>34.47</v>
+      </c>
+      <c r="D15" s="3">
+        <v>34.64</v>
+      </c>
+      <c r="E15" s="3">
+        <v>33.869999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="8">
+        <v>40.54</v>
+      </c>
+      <c r="D16" s="3">
+        <v>39.869999999999997</v>
+      </c>
+      <c r="E16" s="3">
+        <v>39.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="9">
+        <v>65.91</v>
+      </c>
+      <c r="D17" s="5">
+        <v>65.239999999999995</v>
+      </c>
+      <c r="E17" s="5">
+        <v>65.28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="9">
+        <v>34.130000000000003</v>
+      </c>
+      <c r="D18" s="5">
+        <v>31.57</v>
+      </c>
+      <c r="E18" s="5">
+        <v>30.97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="9">
+        <v>25.62</v>
+      </c>
+      <c r="D19" s="5">
+        <v>25.7</v>
+      </c>
+      <c r="E19" s="5">
+        <v>25.74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C20" s="8">
+        <v>66.12</v>
+      </c>
+      <c r="D20" s="3">
+        <v>63.43</v>
+      </c>
+      <c r="E20" s="3">
+        <v>64.02</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="8">
+        <v>38.229999999999997</v>
+      </c>
+      <c r="D21" s="3">
+        <v>37.119999999999997</v>
+      </c>
+      <c r="E21" s="3">
+        <v>38.049999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="8">
+        <v>50.33</v>
+      </c>
+      <c r="D22" s="3">
+        <v>49.98</v>
+      </c>
+      <c r="E22" s="3">
+        <v>49.69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="9">
+        <v>77.02</v>
+      </c>
+      <c r="D23" s="5">
+        <v>76.849999999999994</v>
+      </c>
+      <c r="E23" s="5">
+        <v>76.73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="9">
+        <v>43</v>
+      </c>
+      <c r="D24" s="5">
+        <v>42.92</v>
+      </c>
+      <c r="E24" s="5">
+        <v>43.43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="9">
+        <v>49.72</v>
+      </c>
+      <c r="D25" s="5">
+        <v>49.92</v>
+      </c>
+      <c r="E25" s="5">
+        <v>49.79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="8">
+        <v>75.13</v>
+      </c>
+      <c r="D26" s="3">
+        <v>74.87</v>
+      </c>
+      <c r="E26" s="3">
+        <v>74.03</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="8">
+        <v>45.56</v>
+      </c>
+      <c r="D27" s="3">
+        <v>44.88</v>
+      </c>
+      <c r="E27" s="3">
+        <v>44.45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C28" s="8">
+        <v>60.86</v>
+      </c>
+      <c r="D28" s="3">
+        <v>60.67</v>
+      </c>
+      <c r="E28" s="3">
+        <v>60.47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C29" s="9">
+        <v>74.62</v>
+      </c>
+      <c r="D29" s="5">
+        <v>75.040000000000006</v>
+      </c>
+      <c r="E29" s="5">
+        <v>75.040000000000006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C30" s="9">
+        <v>43.34</v>
+      </c>
+      <c r="D30" s="5">
+        <v>42.41</v>
+      </c>
+      <c r="E30" s="5">
+        <v>41.98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C31" s="9">
+        <v>60.66</v>
+      </c>
+      <c r="D31" s="5">
+        <v>60.44</v>
+      </c>
+      <c r="E31" s="5">
+        <v>60.27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="8">
+        <v>78.489999999999995</v>
+      </c>
+      <c r="D32" s="3">
+        <v>77.819999999999993</v>
+      </c>
+      <c r="E32" s="3">
+        <v>77.95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C33" s="8">
+        <v>45.48</v>
+      </c>
+      <c r="D33" s="3">
+        <v>45.39</v>
+      </c>
+      <c r="E33" s="3">
+        <v>44.54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C34" s="8">
+        <v>51.25</v>
+      </c>
+      <c r="D34" s="3">
+        <v>51.04</v>
+      </c>
+      <c r="E34" s="3">
+        <v>50.45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C35" s="9">
+        <v>78.87</v>
+      </c>
+      <c r="D35" s="5">
+        <v>78.959999999999994</v>
+      </c>
+      <c r="E35" s="5">
+        <v>78.11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C36" s="9">
+        <v>47.78</v>
+      </c>
+      <c r="D36" s="5">
+        <v>46.93</v>
+      </c>
+      <c r="E36" s="5">
+        <v>46.42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C37" s="9">
+        <v>58.55</v>
+      </c>
+      <c r="D37" s="5">
+        <v>58.49</v>
+      </c>
+      <c r="E37" s="5">
+        <v>58.43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C38" s="8">
+        <v>76.09</v>
+      </c>
+      <c r="D38" s="3">
+        <v>76.77</v>
+      </c>
+      <c r="E38" s="3">
+        <v>76.260000000000005</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C39" s="8">
+        <v>44.8</v>
+      </c>
+      <c r="D39" s="3">
+        <v>45.22</v>
+      </c>
+      <c r="E39" s="3">
+        <v>44.8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C40" s="8">
+        <v>62.35</v>
+      </c>
+      <c r="D40" s="3">
+        <v>62.49</v>
+      </c>
+      <c r="E40" s="3">
+        <v>62.26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C41" s="9">
+        <v>76.81</v>
+      </c>
+      <c r="D41" s="5">
+        <v>76.22</v>
+      </c>
+      <c r="E41" s="5">
+        <v>75.510000000000005</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C42" s="9">
+        <v>42.58</v>
+      </c>
+      <c r="D42" s="5">
+        <v>42.32</v>
+      </c>
+      <c r="E42" s="5">
+        <v>42.92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C43" s="9">
+        <v>56.25</v>
+      </c>
+      <c r="D43" s="5">
+        <v>56.54</v>
+      </c>
+      <c r="E43" s="5">
+        <v>56.2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C44" s="8">
+        <v>77.78</v>
+      </c>
+      <c r="D44" s="3">
+        <v>78.37</v>
+      </c>
+      <c r="E44" s="3">
+        <v>78.2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C45" s="8">
+        <v>47.35</v>
+      </c>
+      <c r="D45" s="3">
+        <v>47.27</v>
+      </c>
+      <c r="E45" s="3">
+        <v>46.59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C46" s="8">
+        <v>65.47</v>
+      </c>
+      <c r="D46" s="3">
+        <v>65.55</v>
+      </c>
+      <c r="E46" s="3">
+        <v>65.040000000000006</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C47" s="9">
+        <v>75.88</v>
+      </c>
+      <c r="D47" s="5">
+        <v>75.459999999999994</v>
+      </c>
+      <c r="E47" s="5">
+        <v>75.34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C48" s="9">
+        <v>44.54</v>
+      </c>
+      <c r="D48" s="5">
+        <v>45.39</v>
+      </c>
+      <c r="E48" s="5">
+        <v>45.39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C49" s="9">
+        <v>66.73</v>
+      </c>
+      <c r="D49" s="5">
+        <v>66.260000000000005</v>
+      </c>
+      <c r="E49" s="5">
+        <v>66.02</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C50" s="8">
+        <v>82.79</v>
+      </c>
+      <c r="D50" s="3">
+        <v>83.21</v>
+      </c>
+      <c r="E50" s="3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C51" s="8">
+        <v>57.42</v>
+      </c>
+      <c r="D51" s="3">
+        <v>56.66</v>
+      </c>
+      <c r="E51" s="3">
+        <v>56.14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C52" s="8">
+        <v>69.62</v>
+      </c>
+      <c r="D52" s="3">
+        <v>69.459999999999994</v>
+      </c>
+      <c r="E52" s="3">
+        <v>69.33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C53" s="9">
+        <v>76.05</v>
+      </c>
+      <c r="D53" s="5">
+        <v>75.55</v>
+      </c>
+      <c r="E53" s="5">
+        <v>75.38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C54" s="9">
+        <v>42.06</v>
+      </c>
+      <c r="D54" s="5">
+        <v>40.53</v>
+      </c>
+      <c r="E54" s="5">
+        <v>41.04</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C55" s="9">
+        <v>46.99</v>
+      </c>
+      <c r="D55" s="5">
+        <v>46.69</v>
+      </c>
+      <c r="E55" s="5">
+        <v>46.51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C56" s="8">
+        <v>81.19</v>
+      </c>
+      <c r="D56" s="3">
+        <v>79.38</v>
+      </c>
+      <c r="E56" s="3">
+        <v>79.12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C57" s="8">
+        <v>55.12</v>
+      </c>
+      <c r="D57" s="3">
+        <v>51.96</v>
+      </c>
+      <c r="E57" s="3">
+        <v>52.9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C58" s="8">
+        <v>61.53</v>
+      </c>
+      <c r="D58" s="3">
+        <v>61.35</v>
+      </c>
+      <c r="E58" s="3">
+        <v>61.31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C59" s="9">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="D59" s="5">
+        <v>80.09</v>
+      </c>
+      <c r="E59" s="5">
+        <v>79.97</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C60" s="9">
+        <v>48.12</v>
+      </c>
+      <c r="D60" s="5">
+        <v>48.38</v>
+      </c>
+      <c r="E60" s="5">
+        <v>46.93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C61" s="9">
+        <v>61.02</v>
+      </c>
+      <c r="D61" s="5">
+        <v>60.99</v>
+      </c>
+      <c r="E61" s="5">
+        <v>60.97</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C62" s="8">
+        <v>83.16</v>
+      </c>
+      <c r="D62" s="3">
+        <v>82.91</v>
+      </c>
+      <c r="E62" s="3">
+        <v>82.66</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C63" s="8">
+        <v>53.5</v>
+      </c>
+      <c r="D63" s="3">
+        <v>55.89</v>
+      </c>
+      <c r="E63" s="3">
+        <v>54.95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C64" s="8">
+        <v>61.56</v>
+      </c>
+      <c r="D64" s="3">
+        <v>61.67</v>
+      </c>
+      <c r="E64" s="3">
+        <v>61.57</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C65" s="9">
+        <v>78.91</v>
+      </c>
+      <c r="D65" s="5">
+        <v>78.790000000000006</v>
+      </c>
+      <c r="E65" s="5">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C66" s="9">
+        <v>51.96</v>
+      </c>
+      <c r="D66" s="5">
+        <v>51.96</v>
+      </c>
+      <c r="E66" s="5">
+        <v>50.34</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C67" s="9">
+        <v>71.81</v>
+      </c>
+      <c r="D67" s="5">
+        <v>71.78</v>
+      </c>
+      <c r="E67" s="5">
+        <v>71.680000000000007</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C68" s="8">
+        <v>82.07</v>
+      </c>
+      <c r="D68" s="3">
+        <v>82.49</v>
+      </c>
+      <c r="E68" s="3">
+        <v>82.37</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C69" s="8">
+        <v>52.65</v>
+      </c>
+      <c r="D69" s="3">
+        <v>52.9</v>
+      </c>
+      <c r="E69" s="3">
+        <v>51.71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C70" s="8">
+        <v>71.52</v>
+      </c>
+      <c r="D70" s="3">
+        <v>71.28</v>
+      </c>
+      <c r="E70" s="3">
+        <v>70.84</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C71" s="9">
+        <v>81.31</v>
+      </c>
+      <c r="D71" s="5">
+        <v>80.81</v>
+      </c>
+      <c r="E71" s="5">
+        <v>80.349999999999994</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="5"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C72" s="9">
+        <v>49.4</v>
+      </c>
+      <c r="D72" s="5">
+        <v>48.81</v>
+      </c>
+      <c r="E72" s="5">
+        <v>48.29</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C73" s="9">
+        <v>62.92</v>
+      </c>
+      <c r="D73" s="5">
+        <v>63.08</v>
+      </c>
+      <c r="E73" s="5">
+        <v>62.98</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C74" s="8">
+        <v>81.36</v>
+      </c>
+      <c r="D74" s="3">
+        <v>81.14</v>
+      </c>
+      <c r="E74" s="3">
+        <v>80.930000000000007</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C75" s="8">
+        <v>51.88</v>
+      </c>
+      <c r="D75" s="3">
+        <v>51.71</v>
+      </c>
+      <c r="E75" s="3">
+        <v>52.05</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
+      <c r="C76" s="8">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="D76" s="3">
+        <v>66.12</v>
+      </c>
+      <c r="E76" s="3">
+        <v>65.989999999999995</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Complete data collection for research"
</commit_message>
<xml_diff>
--- a/Research/Results/PROMPTS/Prompt.xlsx
+++ b/Research/Results/PROMPTS/Prompt.xlsx
@@ -8,16 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osins\Desktop\AMU-Master-Thesis-Project\Research\Results\PROMPTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5469067D-93A4-4217-87FD-0EAF0FFD052A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65FC422-6D38-4E62-8CF9-75E106E4F0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="0" windowWidth="13785" windowHeight="15585" tabRatio="592" xr2:uid="{50ED6178-4609-4BB2-9EEF-E5C268DCCA04}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="592" firstSheet="5" activeTab="5" xr2:uid="{50ED6178-4609-4BB2-9EEF-E5C268DCCA04}"/>
   </bookViews>
   <sheets>
-    <sheet name="Prompts" sheetId="5" r:id="rId1"/>
-    <sheet name="Step2" sheetId="7" r:id="rId2"/>
-    <sheet name="Step3" sheetId="9" r:id="rId3"/>
-    <sheet name="Step4" sheetId="8" r:id="rId4"/>
-    <sheet name="PromptMapper" sheetId="6" r:id="rId5"/>
+    <sheet name="1-Prompt" sheetId="5" r:id="rId1"/>
+    <sheet name="1-Results" sheetId="10" r:id="rId2"/>
+    <sheet name="2-Adjective" sheetId="7" r:id="rId3"/>
+    <sheet name="2-Results" sheetId="11" r:id="rId4"/>
+    <sheet name="3-Separator" sheetId="9" r:id="rId5"/>
+    <sheet name="3-Results" sheetId="12" r:id="rId6"/>
+    <sheet name="4-Contamination" sheetId="8" r:id="rId7"/>
+    <sheet name="4-Results" sheetId="13" r:id="rId8"/>
+    <sheet name="PromptMapper" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="82">
   <si>
     <t>Helpful information from the internet for solving the task:</t>
   </si>
@@ -238,6 +242,54 @@
   </si>
   <si>
     <t>(*)</t>
+  </si>
+  <si>
+    <t>"1"</t>
+  </si>
+  <si>
+    <t>"2"</t>
+  </si>
+  <si>
+    <t>"3"</t>
+  </si>
+  <si>
+    <t>"4"</t>
+  </si>
+  <si>
+    <t>"5"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference:  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concept:    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Info:       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Context:    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">null        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WebContext: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data:       </t>
+  </si>
+  <si>
+    <t>Prompt</t>
+  </si>
+  <si>
+    <t>win</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infomative concept: </t>
   </si>
 </sst>
 </file>
@@ -683,11 +735,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{742E4177-CA9C-4411-B8C3-65C6D789DE87}">
   <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,20 +785,20 @@
       <c r="J1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="1">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1">
-        <v>3</v>
-      </c>
-      <c r="N1" s="1">
-        <v>4</v>
-      </c>
-      <c r="O1" s="1">
-        <v>5</v>
+      <c r="K1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4281,14 +4333,186 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C272FE7-9E1D-4780-9EE9-E68F3FA3EEAE}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>656</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E954FFCE-6705-4E93-BCE9-A45F683F8AD8}">
   <dimension ref="A1:R76"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8574,7 +8798,212 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{325E3796-E238-4C44-9800-A122A886F49B}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>743</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467AFD9F-315E-4818-998D-C74A3ADBF2AC}">
   <dimension ref="A1:H76"/>
   <sheetViews>
@@ -10573,7 +11002,99 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703D1AD7-2823-4012-9764-5374370947CD}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2">
+        <v>29</v>
+      </c>
+      <c r="C2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>337</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B9A7D6B-CAE5-41B4-8E9A-54CA3E2B940F}">
   <dimension ref="A1:E76"/>
   <sheetViews>
@@ -11890,7 +12411,69 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A11CD7C-345A-4448-B956-73ABA109091F}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2">
+        <v>46</v>
+      </c>
+      <c r="C2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E38E54-7E1A-4CFD-B06C-07A9872AAA5D}">
   <dimension ref="A1:B5"/>
   <sheetViews>

</xml_diff>